<commit_message>
Extended model a bit
</commit_message>
<xml_diff>
--- a/MA case analysis.xlsx
+++ b/MA case analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mserviciosrc-my.sharepoint.com/personal/lmelahn_lcred_org/Documents/COVID/MA-Covid-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{73E9C425-0FEB-9D45-862D-63319681AE9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F1182664-B9F9-D047-AAE2-DCB640B1D6AA}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{73E9C425-0FEB-9D45-862D-63319681AE9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B28B5990-4B57-5740-9948-FB5BFC85D01B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -106,6 +106,9 @@
   <si>
     <t>Daily Deaths Model *20</t>
   </si>
+  <si>
+    <t>Model (deaths/day)</t>
+  </si>
 </sst>
 </file>
 
@@ -148,7 +151,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -163,6 +166,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -316,10 +322,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Massachussets!$O$2:$O$47</c:f>
+              <c:f>Massachussets!$O$2:$O$70</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>43908</c:v>
                 </c:pt>
@@ -457,16 +463,85 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>43953</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43960</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43961</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>43962</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>43963</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43964</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>43965</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>43967</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>43968</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>43969</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>43970</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>43971</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>43972</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>43973</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>43974</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>43975</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>43976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Massachussets!$P$2:$P$47</c:f>
+              <c:f>Massachussets!$P$2:$P$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -651,10 +726,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Massachussets!$O$2:$O$47</c:f>
+              <c:f>Massachussets!$O$2:$O$70</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>43908</c:v>
                 </c:pt>
@@ -792,16 +867,85 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>43953</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43960</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43961</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>43962</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>43963</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43964</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>43965</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>43967</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>43968</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>43969</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>43970</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>43971</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>43972</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>43973</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>43974</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>43975</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>43976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Massachussets!$Q$2:$Q$47</c:f>
+              <c:f>Massachussets!$Q$2:$Q$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -978,10 +1122,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Massachussets!$O$2:$O$47</c:f>
+              <c:f>Massachussets!$O$2:$O$70</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>43908</c:v>
                 </c:pt>
@@ -1119,16 +1263,85 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>43953</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43960</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43961</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>43962</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>43963</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43964</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>43965</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>43967</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>43968</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>43969</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>43970</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>43971</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>43972</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>43973</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>43974</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>43975</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>43976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Massachussets!$R$2:$R$47</c:f>
+              <c:f>Massachussets!$R$2:$R$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>6.4120156502429433</c:v>
                 </c:pt>
@@ -1266,6 +1479,75 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>4096.1318945103394</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4186.4651018128388</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4267.602263685063</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4339.880151630472</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4403.7365402390569</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4459.6886558109718</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4508.3116757407624</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4550.2180998549557</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4586.0386735132643</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4616.4053824553284</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4641.9368732461489</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4663.2264916951817</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4680.8329838880854</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4695.2737772915661</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4707.0206571424833</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4716.4975779999741</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4724.080301773226</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4730.0975298275926</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4734.8331947035704</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4738.5295925171422</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4741.391065835136</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4743.5879843497569</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4745.2608129651326</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4746.524100468635</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1305,10 +1587,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Massachussets!$O$2:$O$47</c:f>
+              <c:f>Massachussets!$O$2:$O$70</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>43908</c:v>
                 </c:pt>
@@ -1446,16 +1728,85 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>43953</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43960</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43961</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>43962</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>43963</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43964</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>43965</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>43966</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>43967</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>43968</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>43969</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>43970</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>43971</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>43972</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>43973</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>43974</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>43975</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>43976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Massachussets!$S$2:$S$47</c:f>
+              <c:f>Massachussets!$S$2:$S$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="1">
                   <c:v>43.93837029243015</c:v>
                 </c:pt>
@@ -1590,6 +1941,75 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>1994.8870136951973</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1806.6641460499886</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1622.7432374444834</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1445.5577589081804</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1277.1277721716979</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1119.0423114382975</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>972.46039859581288</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>838.12848228386429</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>716.41147316617207</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>607.33417884128357</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>510.62981581640997</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>425.79236898065574</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>352.12984385807431</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>288.81586806961423</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>234.93759701834279</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>189.53841714981536</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>151.65447546503856</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>120.34456108733139</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>94.713297519556363</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>73.927956271436415</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>57.229466359876824</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>43.938370292416948</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>33.456572307513852</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>25.265750070047943</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2425,23 +2845,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{48D865E2-D08D-CC4B-A5A5-2BC248F5DA8C}" name="Table26" displayName="Table26" ref="A1:G47" totalsRowShown="0">
-  <autoFilter ref="A1:G47" xr:uid="{21911FD9-E9A7-7B4E-AA91-03E566661BC3}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{39A5DFED-1B78-7E47-AC29-6651F47201A9}" name="Date of Death" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{D2CBDB34-DDA1-9F49-AF6D-641094478C0F}" name="Time" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{48D865E2-D08D-CC4B-A5A5-2BC248F5DA8C}" name="Table26" displayName="Table26" ref="A1:H74" totalsRowShown="0">
+  <autoFilter ref="A1:H74" xr:uid="{21911FD9-E9A7-7B4E-AA91-03E566661BC3}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{39A5DFED-1B78-7E47-AC29-6651F47201A9}" name="Date of Death" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{D2CBDB34-DDA1-9F49-AF6D-641094478C0F}" name="Time" dataDxfId="11">
       <calculatedColumnFormula>A2-A$2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{C8EE336B-20C3-2246-910B-AF1DB6248AD7}" name="New Deaths"/>
     <tableColumn id="3" xr3:uid="{C1DC7C41-39B7-0549-A511-08ED5BD187E3}" name="Running Total"/>
-    <tableColumn id="4" xr3:uid="{FA5D296B-F3F7-984E-87F9-6DC88F8FABE0}" name="Deaths (normalized)" dataDxfId="9">
+    <tableColumn id="4" xr3:uid="{FA5D296B-F3F7-984E-87F9-6DC88F8FABE0}" name="Deaths (normalized)" dataDxfId="10">
       <calculatedColumnFormula>Table26[[#This Row],[New Deaths]]/MAX(Table26[New Deaths])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F786D82B-4E95-4A44-999E-055BE7FA65F1}" name="Running Total (normalized)" dataDxfId="8">
+    <tableColumn id="5" xr3:uid="{F786D82B-4E95-4A44-999E-055BE7FA65F1}" name="Running Total (normalized)" dataDxfId="9">
       <calculatedColumnFormula>Table26[[#This Row],[Running Total]]/MAX(Table26[Running Total])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{02B4EB61-1F0A-7145-8FE5-CE2A0884B2FB}" name="Model (deaths)" dataDxfId="7">
+    <tableColumn id="12" xr3:uid="{02B4EB61-1F0A-7145-8FE5-CE2A0884B2FB}" name="Model (deaths)" dataDxfId="8">
       <calculatedColumnFormula>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{7E3E1C27-B544-574D-A6B9-FDBD2E213244}" name="Model (deaths/day)" dataDxfId="7">
+      <calculatedColumnFormula>G2-G1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2461,8 +2884,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4A3EC810-A7B9-E347-9B79-6E99EDD0658A}" name="Table9" displayName="Table9" ref="O1:S47" totalsRowShown="0">
-  <autoFilter ref="O1:S47" xr:uid="{8A567930-1BEC-2B42-8586-CA71B39AA169}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4A3EC810-A7B9-E347-9B79-6E99EDD0658A}" name="Table9" displayName="Table9" ref="O1:S70" totalsRowShown="0">
+  <autoFilter ref="O1:S70" xr:uid="{8A567930-1BEC-2B42-8586-CA71B39AA169}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A915EA15-2EFD-014C-B345-428AF1988EE3}" name="Date" dataDxfId="4">
       <calculatedColumnFormula>Table26[[#This Row],[Date of Death]]</calculatedColumnFormula>
@@ -2477,7 +2900,7 @@
       <calculatedColumnFormula>Table26[[#This Row],[Model (deaths)]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{C947925D-F742-9C48-8E43-A291681642B4}" name="Daily Deaths Model *20" dataDxfId="0">
-      <calculatedColumnFormula>Table9[[#This Row],[Deaths Model]]-R1</calculatedColumnFormula>
+      <calculatedColumnFormula>Table26[[#This Row],[Model (deaths/day)]]*20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2747,9 +3170,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48ED21C7-CBD5-CB48-9B6A-6B58F98A2F4A}">
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:S74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="J22" workbookViewId="0">
+      <selection activeCell="P58" sqref="P58"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2786,6 +3211,9 @@
       <c r="G1" t="s">
         <v>21</v>
       </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
       <c r="J1" t="s">
         <v>6</v>
       </c>
@@ -2837,6 +3265,7 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>6.4120156502429433</v>
       </c>
+      <c r="H2" s="2"/>
       <c r="J2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2890,6 +3319,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>8.6089341648644506</v>
       </c>
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H33" si="1">G3-G2</f>
+        <v>2.1969185146215073</v>
+      </c>
       <c r="J3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2916,7 +3349,7 @@
         <v>8.6089341648644506</v>
       </c>
       <c r="S3" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R2)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>43.93837029243015</v>
       </c>
     </row>
@@ -2946,6 +3379,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>11.470407482857341</v>
       </c>
+      <c r="H4" s="2">
+        <f t="shared" si="1"/>
+        <v>2.8614733179928908</v>
+      </c>
       <c r="J4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2972,7 +3409,7 @@
         <v>11.470407482857341</v>
       </c>
       <c r="S4" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R3)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>57.229466359857817</v>
       </c>
     </row>
@@ -3002,6 +3439,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>15.16680529642926</v>
       </c>
+      <c r="H5" s="2">
+        <f t="shared" si="1"/>
+        <v>3.6963978135719184</v>
+      </c>
       <c r="J5" s="2" t="s">
         <v>5</v>
       </c>
@@ -3028,7 +3469,7 @@
         <v>15.16680529642926</v>
       </c>
       <c r="S5" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R4)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>73.927956271438376</v>
       </c>
     </row>
@@ -3058,6 +3499,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>19.90247017240744</v>
       </c>
+      <c r="H6" s="2">
+        <f t="shared" si="1"/>
+        <v>4.7356648759781805</v>
+      </c>
       <c r="J6" s="2" t="s">
         <v>7</v>
       </c>
@@ -3084,7 +3529,7 @@
         <v>19.90247017240744</v>
       </c>
       <c r="S6" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R5)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>94.713297519563611</v>
       </c>
     </row>
@@ -3114,6 +3559,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>25.919698226774216</v>
       </c>
+      <c r="H7" s="2">
+        <f t="shared" si="1"/>
+        <v>6.0172280543667753</v>
+      </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="O7" s="1">
@@ -3133,7 +3582,7 @@
         <v>25.919698226774216</v>
       </c>
       <c r="S7" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R6)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>120.34456108733551</v>
       </c>
     </row>
@@ -3163,6 +3612,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>33.502422000026378</v>
       </c>
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
+        <v>7.5827237732521624</v>
+      </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="O8" s="1">
@@ -3182,7 +3635,7 @@
         <v>33.502422000026378</v>
       </c>
       <c r="S8" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R7)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>151.65447546504325</v>
       </c>
     </row>
@@ -3212,6 +3665,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>42.979342857516379</v>
       </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>9.4769208574900006</v>
+      </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="O9" s="1">
@@ -3231,7 +3688,7 @@
         <v>42.979342857516379</v>
       </c>
       <c r="S9" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R8)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>189.53841714980001</v>
       </c>
     </row>
@@ -3261,6 +3718,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>54.726222708434371</v>
       </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>11.746879850917992</v>
+      </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="O10" s="1">
@@ -3280,7 +3741,7 @@
         <v>54.726222708434371</v>
       </c>
       <c r="S10" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R9)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>234.93759701835984</v>
       </c>
     </row>
@@ -3310,6 +3771,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>69.167016111914492</v>
       </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>14.440793403480122</v>
+      </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="O11" s="1">
@@ -3329,7 +3794,7 @@
         <v>69.167016111914492</v>
       </c>
       <c r="S11" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R10)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>288.8158680696024</v>
       </c>
     </row>
@@ -3359,6 +3824,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>86.77350830481808</v>
       </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>17.606492192903588</v>
+      </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="O12" s="1">
@@ -3378,7 +3847,7 @@
         <v>86.77350830481808</v>
       </c>
       <c r="S12" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R11)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>352.12984385807175</v>
       </c>
     </row>
@@ -3408,6 +3877,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>108.06312675385117</v>
       </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>21.289618449033085</v>
+      </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="O13" s="1">
@@ -3427,7 +3900,7 @@
         <v>108.06312675385117</v>
       </c>
       <c r="S13" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R12)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>425.79236898066171</v>
       </c>
     </row>
@@ -3457,6 +3930,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>133.59461754467122</v>
       </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>25.531490790820058</v>
+      </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="O14" s="1">
@@ -3476,7 +3953,7 @@
         <v>133.59461754467122</v>
       </c>
       <c r="S14" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R13)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>510.62981581640116</v>
       </c>
     </row>
@@ -3506,6 +3983,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>163.96132648673623</v>
       </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>30.366708942065003</v>
+      </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="O15" s="1">
@@ -3525,7 +4006,7 @@
         <v>163.96132648673623</v>
       </c>
       <c r="S15" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R14)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>607.33417884130006</v>
       </c>
     </row>
@@ -3555,6 +4036,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>199.78190014504457</v>
       </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>35.820573658308348</v>
+      </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="O16" s="1">
@@ -3574,7 +4059,7 @@
         <v>199.78190014504457</v>
       </c>
       <c r="S16" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R15)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>716.41147316616696</v>
       </c>
     </row>
@@ -3604,6 +4089,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>241.68832425923688</v>
       </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>41.906424114192305</v>
+      </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="O17" s="1">
@@ -3623,7 +4112,7 @@
         <v>241.68832425923688</v>
       </c>
       <c r="S17" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R16)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>838.1284822838461</v>
       </c>
     </row>
@@ -3653,6 +4142,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>290.31134418902798</v>
       </c>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>48.623019929791099</v>
+      </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="O18" s="1">
@@ -3672,7 +4165,7 @@
         <v>290.31134418902798</v>
       </c>
       <c r="S18" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R17)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>972.46039859582197</v>
       </c>
     </row>
@@ -3702,6 +4195,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>346.26345976094302</v>
       </c>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>55.952115571915044</v>
+      </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="O19" s="1">
@@ -3721,7 +4218,7 @@
         <v>346.26345976094302</v>
       </c>
       <c r="S19" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R18)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>1119.0423114383009</v>
       </c>
     </row>
@@ -3751,6 +4248,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>410.11984836952757</v>
       </c>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>63.856388608584552</v>
+      </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="O20" s="1">
@@ -3770,7 +4271,7 @@
         <v>410.11984836952757</v>
       </c>
       <c r="S20" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R19)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>1277.127772171691</v>
       </c>
     </row>
@@ -3800,6 +4301,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>482.39773631493733</v>
       </c>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>72.277887945409759</v>
+      </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="O21" s="1">
@@ -3819,7 +4324,7 @@
         <v>482.39773631493733</v>
       </c>
       <c r="S21" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R20)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>1445.5577589081952</v>
       </c>
     </row>
@@ -3849,6 +4354,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>563.53489818716093</v>
       </c>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>81.137161872223601</v>
+      </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="O22" s="1">
@@ -3868,7 +4377,7 @@
         <v>563.53489818716093</v>
       </c>
       <c r="S22" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R21)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>1622.743237444472</v>
       </c>
     </row>
@@ -3898,6 +4407,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>653.86810548966105</v>
       </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>90.333207302500114</v>
+      </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="O23" s="1">
@@ -3917,7 +4430,7 @@
         <v>653.86810548966105</v>
       </c>
       <c r="S23" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R22)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>1806.6641460500023</v>
       </c>
     </row>
@@ -3947,6 +4460,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>753.61245617442069</v>
       </c>
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
+        <v>99.744350684759638</v>
+      </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="O24" s="1">
@@ -3966,7 +4483,7 @@
         <v>753.61245617442069</v>
       </c>
       <c r="S24" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R23)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>1994.8870136951928</v>
       </c>
     </row>
@@ -3996,6 +4513,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>862.8425846063825</v>
       </c>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>109.23012843196182</v>
+      </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="O25" s="1">
@@ -4015,7 +4536,7 @@
         <v>862.8425846063825</v>
       </c>
       <c r="S25" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R24)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>2184.6025686392363</v>
       </c>
     </row>
@@ -4045,6 +4566,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>981.47676679739618</v>
       </c>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>118.63418219101368</v>
+      </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="O26" s="1">
@@ -4064,7 +4589,7 @@
         <v>981.47676679739618</v>
       </c>
       <c r="S26" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R25)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>2372.6836438202736</v>
       </c>
     </row>
@@ -4094,6 +4619,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>1109.2648915735372</v>
       </c>
+      <c r="H27" s="2">
+        <f t="shared" si="1"/>
+        <v>127.78812477614099</v>
+      </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="O27" s="1">
@@ -4113,7 +4642,7 @@
         <v>1109.2648915735372</v>
       </c>
       <c r="S27" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R26)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>2555.7624955228198</v>
       </c>
     </row>
@@ -4143,6 +4672,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>1245.781161533868</v>
       </c>
+      <c r="H28" s="2">
+        <f t="shared" si="1"/>
+        <v>136.51626996033087</v>
+      </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="O28" s="1">
@@ -4162,7 +4695,7 @@
         <v>1245.781161533868</v>
       </c>
       <c r="S28" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R27)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>2730.3253992066175</v>
       </c>
     </row>
@@ -4192,6 +4725,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>1390.422219601202</v>
       </c>
+      <c r="H29" s="2">
+        <f t="shared" si="1"/>
+        <v>144.64105806733392</v>
+      </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="O29" s="1">
@@ -4211,7 +4748,7 @@
         <v>1390.422219601202</v>
       </c>
       <c r="S29" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R28)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>2892.8211613466783</v>
       </c>
     </row>
@@ -4241,6 +4778,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>1542.4111738510423</v>
       </c>
+      <c r="H30" s="2">
+        <f t="shared" si="1"/>
+        <v>151.98895424984039</v>
+      </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="O30" s="1">
@@ -4260,7 +4801,7 @@
         <v>1542.4111738510423</v>
       </c>
       <c r="S30" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R29)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>3039.7790849968078</v>
       </c>
     </row>
@@ -4290,6 +4831,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>1700.8077260319676</v>
       </c>
+      <c r="H31" s="2">
+        <f t="shared" si="1"/>
+        <v>158.39655218092526</v>
+      </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="O31" s="1">
@@ -4309,7 +4854,7 @@
         <v>1700.8077260319676</v>
       </c>
       <c r="S31" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R30)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>3167.9310436185051</v>
       </c>
     </row>
@@ -4339,6 +4884,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>1864.5243128004536</v>
       </c>
+      <c r="H32" s="2">
+        <f t="shared" si="1"/>
+        <v>163.71658676848597</v>
+      </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="O32" s="1">
@@ -4358,7 +4907,7 @@
         <v>1864.5243128004536</v>
       </c>
       <c r="S32" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R31)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>3274.3317353697194</v>
       </c>
     </row>
@@ -4388,6 +4937,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>2032.3478613851698</v>
       </c>
+      <c r="H33" s="2">
+        <f t="shared" si="1"/>
+        <v>167.82354858471626</v>
+      </c>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="O33" s="1">
@@ -4407,7 +4960,7 @@
         <v>2032.3478613851698</v>
       </c>
       <c r="S33" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R32)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>3356.4709716943253</v>
       </c>
     </row>
@@ -4437,6 +4990,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>2202.9664631897517</v>
       </c>
+      <c r="H34" s="2">
+        <f t="shared" ref="H34:H65" si="2">G34-G33</f>
+        <v>170.61860180458189</v>
+      </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="O34" s="1">
@@ -4456,7 +5013,7 @@
         <v>2202.9664631897517</v>
       </c>
       <c r="S34" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R33)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>3412.3720360916377</v>
       </c>
     </row>
@@ -4486,6 +5043,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>2375</v>
       </c>
+      <c r="H35" s="2">
+        <f t="shared" si="2"/>
+        <v>172.03353681024828</v>
+      </c>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="O35" s="1">
@@ -4505,7 +5066,7 @@
         <v>2375</v>
       </c>
       <c r="S35" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R34)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>3440.6707362049656</v>
       </c>
     </row>
@@ -4535,6 +5096,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>2547.0335368102483</v>
       </c>
+      <c r="H36" s="2">
+        <f t="shared" si="2"/>
+        <v>172.03353681024828</v>
+      </c>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="O36" s="1">
@@ -4554,7 +5119,7 @@
         <v>2547.0335368102483</v>
       </c>
       <c r="S36" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R35)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>3440.6707362049656</v>
       </c>
     </row>
@@ -4584,6 +5149,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>2717.6521386148302</v>
       </c>
+      <c r="H37" s="2">
+        <f t="shared" si="2"/>
+        <v>170.61860180458189</v>
+      </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="O37" s="1">
@@ -4603,7 +5172,7 @@
         <v>2717.6521386148302</v>
       </c>
       <c r="S37" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R36)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>3412.3720360916377</v>
       </c>
     </row>
@@ -4633,6 +5202,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>2885.4756871995464</v>
       </c>
+      <c r="H38" s="2">
+        <f t="shared" si="2"/>
+        <v>167.82354858471626</v>
+      </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="O38" s="1">
@@ -4652,7 +5225,7 @@
         <v>2885.4756871995464</v>
       </c>
       <c r="S38" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R37)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>3356.4709716943253</v>
       </c>
     </row>
@@ -4682,6 +5255,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>3049.1922739680322</v>
       </c>
+      <c r="H39" s="2">
+        <f t="shared" si="2"/>
+        <v>163.71658676848574</v>
+      </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="O39" s="1">
@@ -4701,7 +5278,7 @@
         <v>3049.1922739680322</v>
       </c>
       <c r="S39" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R38)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>3274.3317353697148</v>
       </c>
     </row>
@@ -4731,6 +5308,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>3207.5888261489577</v>
       </c>
+      <c r="H40" s="2">
+        <f t="shared" si="2"/>
+        <v>158.39655218092548</v>
+      </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="O40" s="1">
@@ -4750,7 +5331,7 @@
         <v>3207.5888261489577</v>
       </c>
       <c r="S40" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R39)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>3167.9310436185096</v>
       </c>
     </row>
@@ -4780,6 +5361,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>3359.577780398798</v>
       </c>
+      <c r="H41" s="2">
+        <f t="shared" si="2"/>
+        <v>151.98895424984039</v>
+      </c>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="O41" s="1">
@@ -4799,7 +5384,7 @@
         <v>3359.577780398798</v>
       </c>
       <c r="S41" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R40)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>3039.7790849968078</v>
       </c>
     </row>
@@ -4829,6 +5414,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>3504.2188384661317</v>
       </c>
+      <c r="H42" s="2">
+        <f t="shared" si="2"/>
+        <v>144.64105806733369</v>
+      </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="O42" s="1">
@@ -4848,7 +5437,7 @@
         <v>3504.2188384661317</v>
       </c>
       <c r="S42" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R41)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>2892.8211613466738</v>
       </c>
     </row>
@@ -4878,6 +5467,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>3640.7351084264628</v>
       </c>
+      <c r="H43" s="2">
+        <f t="shared" si="2"/>
+        <v>136.5162699603311</v>
+      </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="O43" s="1">
@@ -4897,7 +5490,7 @@
         <v>3640.7351084264628</v>
       </c>
       <c r="S43" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R42)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>2730.325399206622</v>
       </c>
     </row>
@@ -4927,6 +5520,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>3768.5232332026039</v>
       </c>
+      <c r="H44" s="2">
+        <f t="shared" si="2"/>
+        <v>127.7881247761411</v>
+      </c>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="O44" s="1">
@@ -4946,7 +5543,7 @@
         <v>3768.5232332026039</v>
       </c>
       <c r="S44" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R43)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>2555.7624955228221</v>
       </c>
     </row>
@@ -4976,6 +5573,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>3887.1574153936176</v>
       </c>
+      <c r="H45" s="2">
+        <f t="shared" si="2"/>
+        <v>118.63418219101368</v>
+      </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="O45" s="1">
@@ -4995,7 +5596,7 @@
         <v>3887.1574153936176</v>
       </c>
       <c r="S45" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R44)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>2372.6836438202736</v>
       </c>
     </row>
@@ -5025,6 +5626,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>3996.3875438255795</v>
       </c>
+      <c r="H46" s="2">
+        <f t="shared" si="2"/>
+        <v>109.23012843196193</v>
+      </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="O46" s="1">
@@ -5044,7 +5649,7 @@
         <v>3996.3875438255795</v>
       </c>
       <c r="S46" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R45)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>2184.6025686392386</v>
       </c>
     </row>
@@ -5074,6 +5679,10 @@
         <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
         <v>4096.1318945103394</v>
       </c>
+      <c r="H47" s="2">
+        <f t="shared" si="2"/>
+        <v>99.744350684759866</v>
+      </c>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
       <c r="O47" s="1">
@@ -5093,12 +5702,841 @@
         <v>4096.1318945103394</v>
       </c>
       <c r="S47" s="2">
-        <f>(Table9[[#This Row],[Deaths Model]]-R46)*20</f>
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
         <v>1994.8870136951973</v>
       </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>43954</v>
+      </c>
+      <c r="B48" s="2">
+        <f t="shared" ref="B48:B54" si="3">A48-A$2</f>
+        <v>46</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4186.4651018128388</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="2"/>
+        <v>90.333207302499432</v>
+      </c>
+      <c r="O48" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43954</v>
+      </c>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4186.4651018128388</v>
+      </c>
+      <c r="S48" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>1806.6641460499886</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>43955</v>
+      </c>
+      <c r="B49" s="2">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4267.602263685063</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="2"/>
+        <v>81.137161872224169</v>
+      </c>
+      <c r="O49" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43955</v>
+      </c>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4267.602263685063</v>
+      </c>
+      <c r="S49" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>1622.7432374444834</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>43956</v>
+      </c>
+      <c r="B50" s="2">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4339.880151630472</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="2"/>
+        <v>72.27788794540902</v>
+      </c>
+      <c r="O50" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43956</v>
+      </c>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4339.880151630472</v>
+      </c>
+      <c r="S50" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>1445.5577589081804</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>43957</v>
+      </c>
+      <c r="B51" s="2">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4403.7365402390569</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="2"/>
+        <v>63.856388608584894</v>
+      </c>
+      <c r="O51" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43957</v>
+      </c>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4403.7365402390569</v>
+      </c>
+      <c r="S51" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>1277.1277721716979</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>43958</v>
+      </c>
+      <c r="B52" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4459.6886558109718</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="2"/>
+        <v>55.952115571914874</v>
+      </c>
+      <c r="O52" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43958</v>
+      </c>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4459.6886558109718</v>
+      </c>
+      <c r="S52" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>1119.0423114382975</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>43959</v>
+      </c>
+      <c r="B53" s="2">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4508.3116757407624</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="2"/>
+        <v>48.623019929790644</v>
+      </c>
+      <c r="O53" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43959</v>
+      </c>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4508.3116757407624</v>
+      </c>
+      <c r="S53" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>972.46039859581288</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>43960</v>
+      </c>
+      <c r="B54" s="2">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4550.2180998549557</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="2"/>
+        <v>41.906424114193214</v>
+      </c>
+      <c r="O54" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43960</v>
+      </c>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4550.2180998549557</v>
+      </c>
+      <c r="S54" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>838.12848228386429</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B55" s="2">
+        <f t="shared" ref="B55:B62" si="4">A55-A$2</f>
+        <v>53</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4586.0386735132643</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" si="2"/>
+        <v>35.820573658308604</v>
+      </c>
+      <c r="O55" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43961</v>
+      </c>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4586.0386735132643</v>
+      </c>
+      <c r="S55" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>716.41147316617207</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>43962</v>
+      </c>
+      <c r="B56" s="2">
+        <f t="shared" si="4"/>
+        <v>54</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4616.4053824553284</v>
+      </c>
+      <c r="H56" s="2">
+        <f t="shared" si="2"/>
+        <v>30.366708942064179</v>
+      </c>
+      <c r="O56" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43962</v>
+      </c>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4616.4053824553284</v>
+      </c>
+      <c r="S56" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>607.33417884128357</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>43963</v>
+      </c>
+      <c r="B57" s="2">
+        <f t="shared" si="4"/>
+        <v>55</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4641.9368732461489</v>
+      </c>
+      <c r="H57" s="2">
+        <f t="shared" si="2"/>
+        <v>25.531490790820499</v>
+      </c>
+      <c r="O57" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43963</v>
+      </c>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4641.9368732461489</v>
+      </c>
+      <c r="S57" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>510.62981581640997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>43964</v>
+      </c>
+      <c r="B58" s="2">
+        <f t="shared" si="4"/>
+        <v>56</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4663.2264916951817</v>
+      </c>
+      <c r="H58" s="2">
+        <f t="shared" si="2"/>
+        <v>21.289618449032787</v>
+      </c>
+      <c r="O58" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43964</v>
+      </c>
+      <c r="Q58" s="2"/>
+      <c r="R58" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4663.2264916951817</v>
+      </c>
+      <c r="S58" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>425.79236898065574</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>43965</v>
+      </c>
+      <c r="B59" s="2">
+        <f t="shared" si="4"/>
+        <v>57</v>
+      </c>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4680.8329838880854</v>
+      </c>
+      <c r="H59" s="2">
+        <f t="shared" si="2"/>
+        <v>17.606492192903715</v>
+      </c>
+      <c r="O59" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43965</v>
+      </c>
+      <c r="Q59" s="2"/>
+      <c r="R59" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4680.8329838880854</v>
+      </c>
+      <c r="S59" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>352.12984385807431</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>43966</v>
+      </c>
+      <c r="B60" s="2">
+        <f t="shared" si="4"/>
+        <v>58</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4695.2737772915661</v>
+      </c>
+      <c r="H60" s="2">
+        <f t="shared" si="2"/>
+        <v>14.440793403480711</v>
+      </c>
+      <c r="O60" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43966</v>
+      </c>
+      <c r="Q60" s="2"/>
+      <c r="R60" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4695.2737772915661</v>
+      </c>
+      <c r="S60" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>288.81586806961423</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>43967</v>
+      </c>
+      <c r="B61" s="2">
+        <f t="shared" si="4"/>
+        <v>59</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4707.0206571424833</v>
+      </c>
+      <c r="H61" s="2">
+        <f t="shared" si="2"/>
+        <v>11.746879850917139</v>
+      </c>
+      <c r="O61" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43967</v>
+      </c>
+      <c r="Q61" s="2"/>
+      <c r="R61" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4707.0206571424833</v>
+      </c>
+      <c r="S61" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>234.93759701834279</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>43968</v>
+      </c>
+      <c r="B62" s="2">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4716.4975779999741</v>
+      </c>
+      <c r="H62" s="2">
+        <f t="shared" si="2"/>
+        <v>9.476920857490768</v>
+      </c>
+      <c r="O62" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43968</v>
+      </c>
+      <c r="Q62" s="2"/>
+      <c r="R62" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4716.4975779999741</v>
+      </c>
+      <c r="S62" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>189.53841714981536</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>43969</v>
+      </c>
+      <c r="B63" s="2">
+        <f t="shared" ref="B63:B69" si="5">A63-A$2</f>
+        <v>61</v>
+      </c>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4724.080301773226</v>
+      </c>
+      <c r="H63" s="2">
+        <f t="shared" si="2"/>
+        <v>7.5827237732519279</v>
+      </c>
+      <c r="O63" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43969</v>
+      </c>
+      <c r="Q63" s="2"/>
+      <c r="R63" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4724.080301773226</v>
+      </c>
+      <c r="S63" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>151.65447546503856</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>43970</v>
+      </c>
+      <c r="B64" s="2">
+        <f t="shared" si="5"/>
+        <v>62</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4730.0975298275926</v>
+      </c>
+      <c r="H64" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0172280543665693</v>
+      </c>
+      <c r="O64" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43970</v>
+      </c>
+      <c r="Q64" s="2"/>
+      <c r="R64" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4730.0975298275926</v>
+      </c>
+      <c r="S64" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>120.34456108733139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>43971</v>
+      </c>
+      <c r="B65" s="2">
+        <f t="shared" si="5"/>
+        <v>63</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4734.8331947035704</v>
+      </c>
+      <c r="H65" s="2">
+        <f t="shared" si="2"/>
+        <v>4.7356648759778182</v>
+      </c>
+      <c r="O65" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43971</v>
+      </c>
+      <c r="Q65" s="2"/>
+      <c r="R65" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4734.8331947035704</v>
+      </c>
+      <c r="S65" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>94.713297519556363</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>43972</v>
+      </c>
+      <c r="B66" s="2">
+        <f t="shared" si="5"/>
+        <v>64</v>
+      </c>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4738.5295925171422</v>
+      </c>
+      <c r="H66" s="2">
+        <f t="shared" ref="H66:H74" si="6">G66-G65</f>
+        <v>3.6963978135718207</v>
+      </c>
+      <c r="O66" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43972</v>
+      </c>
+      <c r="Q66" s="2"/>
+      <c r="R66" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4738.5295925171422</v>
+      </c>
+      <c r="S66" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>73.927956271436415</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>43973</v>
+      </c>
+      <c r="B67" s="2">
+        <f t="shared" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4741.391065835136</v>
+      </c>
+      <c r="H67" s="2">
+        <f t="shared" si="6"/>
+        <v>2.8614733179938412</v>
+      </c>
+      <c r="O67" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43973</v>
+      </c>
+      <c r="Q67" s="2"/>
+      <c r="R67" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4741.391065835136</v>
+      </c>
+      <c r="S67" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>57.229466359876824</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>43974</v>
+      </c>
+      <c r="B68" s="2">
+        <f t="shared" si="5"/>
+        <v>66</v>
+      </c>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4743.5879843497569</v>
+      </c>
+      <c r="H68" s="2">
+        <f t="shared" si="6"/>
+        <v>2.1969185146208474</v>
+      </c>
+      <c r="O68" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43974</v>
+      </c>
+      <c r="Q68" s="2"/>
+      <c r="R68" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4743.5879843497569</v>
+      </c>
+      <c r="S68" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>43.938370292416948</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>43975</v>
+      </c>
+      <c r="B69" s="2">
+        <f t="shared" si="5"/>
+        <v>67</v>
+      </c>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4745.2608129651326</v>
+      </c>
+      <c r="H69" s="2">
+        <f t="shared" si="6"/>
+        <v>1.6728286153756926</v>
+      </c>
+      <c r="O69" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43975</v>
+      </c>
+      <c r="Q69" s="2"/>
+      <c r="R69" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4745.2608129651326</v>
+      </c>
+      <c r="S69" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>33.456572307513852</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>43976</v>
+      </c>
+      <c r="B70" s="2">
+        <f t="shared" ref="B70:B74" si="7">A70-A$2</f>
+        <v>68</v>
+      </c>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4746.524100468635</v>
+      </c>
+      <c r="H70" s="2">
+        <f t="shared" si="6"/>
+        <v>1.2632875035023972</v>
+      </c>
+      <c r="O70" s="1">
+        <f>Table26[[#This Row],[Date of Death]]</f>
+        <v>43976</v>
+      </c>
+      <c r="Q70" s="2"/>
+      <c r="R70" s="2">
+        <f>Table26[[#This Row],[Model (deaths)]]</f>
+        <v>4746.524100468635</v>
+      </c>
+      <c r="S70" s="2">
+        <f>Table26[[#This Row],[Model (deaths/day)]]*20</f>
+        <v>25.265750070047943</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>43977</v>
+      </c>
+      <c r="B71" s="2">
+        <f t="shared" si="7"/>
+        <v>69</v>
+      </c>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4747.4702639938905</v>
+      </c>
+      <c r="H71" s="2">
+        <f t="shared" si="6"/>
+        <v>0.94616352525554248</v>
+      </c>
+      <c r="O71" s="1"/>
+      <c r="Q71" s="2"/>
+      <c r="R71" s="2"/>
+      <c r="S71" s="2"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>43978</v>
+      </c>
+      <c r="B72" s="2">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4748.1730829292883</v>
+      </c>
+      <c r="H72" s="2">
+        <f t="shared" si="6"/>
+        <v>0.70281893539777229</v>
+      </c>
+      <c r="O72" s="1"/>
+      <c r="Q72" s="2"/>
+      <c r="R72" s="2"/>
+      <c r="S72" s="2"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>43979</v>
+      </c>
+      <c r="B73" s="2">
+        <f t="shared" si="7"/>
+        <v>71</v>
+      </c>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4748.6908494380332</v>
+      </c>
+      <c r="H73" s="2">
+        <f t="shared" si="6"/>
+        <v>0.5177665087448986</v>
+      </c>
+      <c r="O73" s="1"/>
+      <c r="Q73" s="2"/>
+      <c r="R73" s="2"/>
+      <c r="S73" s="2"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>43980</v>
+      </c>
+      <c r="B74" s="2">
+        <f t="shared" si="7"/>
+        <v>72</v>
+      </c>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2">
+        <f>$K$4*NORMDIST(Table26[[#This Row],[Time]],$K$2,$K$3,1)</f>
+        <v>4749.0691506260637</v>
+      </c>
+      <c r="H74" s="2">
+        <f t="shared" si="6"/>
+        <v>0.37830118803049118</v>
+      </c>
+      <c r="O74" s="1"/>
+      <c r="Q74" s="2"/>
+      <c r="R74" s="2"/>
+      <c r="S74" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
   <tableParts count="3">
     <tablePart r:id="rId2"/>

</xml_diff>